<commit_message>
added mapping portions, shape files, etc
</commit_message>
<xml_diff>
--- a/photogrammetry/data/siteCoordinates.xlsx
+++ b/photogrammetry/data/siteCoordinates.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iancombs/Documents/GitHub/photogrammetryNOAA/photogrammetry/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{452845F5-0194-094E-BC79-264A177D9A30}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56B0C389-3C20-2741-B5E9-86C216F0612B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17240" yWindow="580" windowWidth="16360" windowHeight="17440" xr2:uid="{6629BE97-6F76-EA48-AE45-A736C90597F0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Lat_Y</t>
   </si>
@@ -60,6 +60,18 @@
   </si>
   <si>
     <t>Site_ID</t>
+  </si>
+  <si>
+    <t>Reef</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>Z</t>
   </si>
 </sst>
 </file>
@@ -411,88 +423,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C324927E-CAF8-4F4E-AA26-4BA23EE9A8E0}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
         <v>24.53116</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>-81.484549999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
         <v>24.530919999999998</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>-81.485439999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4">
         <v>24.540700000000001</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>-81.443870000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5">
         <v>24.54045</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>-81.445419999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
         <v>24.527660000000001</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>-81.497789999999995</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B7">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
         <v>24.5274</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>-81.49897</v>
       </c>
     </row>

</xml_diff>